<commit_message>
added some notes to rubic
</commit_message>
<xml_diff>
--- a/Graphics II Project Rubric.xlsx
+++ b/Graphics II Project Rubric.xlsx
@@ -114,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="83">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -412,6 +412,9 @@
   </si>
   <si>
     <t>James Bean - tutor, helped with understanding Vertext shaders and Pixel shaders</t>
+  </si>
+  <si>
+    <t>II</t>
   </si>
 </sst>
 </file>
@@ -932,8 +935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A97" sqref="A97"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1065,7 +1068,7 @@
       </c>
       <c r="I4" s="5">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 22, 22, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J4" s="5">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 22, 22, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91))</f>
@@ -1077,7 +1080,7 @@
       </c>
       <c r="L4" s="9">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1167,7 +1170,9 @@
       <c r="D7" s="5">
         <v>4</v>
       </c>
-      <c r="E7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="F7" s="3"/>
       <c r="G7" s="8">
         <f t="shared" si="0"/>
@@ -1210,7 +1215,7 @@
       </c>
       <c r="I8" s="9">
         <f>I4+IF(I4 &lt; 22, IF(H10+I4 &gt; 22, 22- I4, H10),0)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J8" s="9">
         <f>J4+IF(J4 &lt; 22, IF(I10+J4 &gt; 22, 22- J4, I10),0)</f>
@@ -1580,7 +1585,9 @@
       <c r="D24" s="5">
         <v>5</v>
       </c>
-      <c r="E24" s="2"/>
+      <c r="E24" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="F24" s="3"/>
       <c r="G24" s="8">
         <f t="shared" si="0"/>
@@ -1721,7 +1728,9 @@
       <c r="D31" s="5">
         <v>3</v>
       </c>
-      <c r="E31" s="2"/>
+      <c r="E31" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="F31" s="3"/>
       <c r="G31" s="8">
         <f t="shared" si="0"/>
@@ -1746,7 +1755,9 @@
       <c r="D32" s="5">
         <v>3</v>
       </c>
-      <c r="E32" s="2"/>
+      <c r="E32" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="F32" s="3"/>
       <c r="G32" s="8">
         <f t="shared" si="0"/>
@@ -1771,11 +1782,15 @@
       <c r="D33" s="5">
         <v>1</v>
       </c>
-      <c r="E33" s="2"/>
-      <c r="F33" s="3"/>
+      <c r="E33" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G33" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
@@ -1796,7 +1811,9 @@
       <c r="D34" s="5">
         <v>1</v>
       </c>
-      <c r="E34" s="2"/>
+      <c r="E34" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="F34" s="3"/>
       <c r="G34" s="8">
         <f t="shared" si="0"/>
@@ -1821,7 +1838,9 @@
       <c r="D35" s="5">
         <v>1</v>
       </c>
-      <c r="E35" s="2"/>
+      <c r="E35" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="F35" s="3"/>
       <c r="G35" s="8">
         <f t="shared" si="0"/>
@@ -1846,7 +1865,9 @@
       <c r="D36" s="5">
         <v>2</v>
       </c>
-      <c r="E36" s="2"/>
+      <c r="E36" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="F36" s="3"/>
       <c r="G36" s="8">
         <f t="shared" ref="G36:G67" si="1" xml:space="preserve"> IF(EXACT(F36,"X"),IF(EXACT(E36,"I"),$B36,IF(EXACT(E36,"II"),$C36,IF(EXACT(E36,"III"),$D36,0))),0)</f>
@@ -2220,7 +2241,9 @@
       <c r="D54" s="5">
         <v>3</v>
       </c>
-      <c r="E54" s="2"/>
+      <c r="E54" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="F54" s="3"/>
       <c r="G54" s="8">
         <f t="shared" si="1"/>
@@ -2245,7 +2268,9 @@
       <c r="D55" s="5">
         <v>3</v>
       </c>
-      <c r="E55" s="2"/>
+      <c r="E55" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="F55" s="3"/>
       <c r="G55" s="8">
         <f t="shared" si="1"/>
@@ -2499,7 +2524,9 @@
       <c r="D67" s="5">
         <v>5</v>
       </c>
-      <c r="E67" s="2"/>
+      <c r="E67" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="F67" s="3"/>
       <c r="G67" s="8">
         <f t="shared" si="1"/>
@@ -2524,7 +2551,9 @@
       <c r="D68" s="5">
         <v>5</v>
       </c>
-      <c r="E68" s="2"/>
+      <c r="E68" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="F68" s="3"/>
       <c r="G68" s="8">
         <f t="shared" ref="G68:G85" si="2" xml:space="preserve"> IF(EXACT(F68,"X"),IF(EXACT(E68,"I"),$B68,IF(EXACT(E68,"II"),$C68,IF(EXACT(E68,"III"),$D68,0))),0)</f>
@@ -3071,7 +3100,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
two viewports on same screen
</commit_message>
<xml_diff>
--- a/Graphics II Project Rubric.xlsx
+++ b/Graphics II Project Rubric.xlsx
@@ -211,7 +211,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="84">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -512,6 +512,9 @@
   </si>
   <si>
     <t>II</t>
+  </si>
+  <si>
+    <t>http://www.braynzarsoft.net/index.php?p=DX11Lessons</t>
   </si>
 </sst>
 </file>
@@ -1032,8 +1035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E91" sqref="E91"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A81" sqref="A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3130,7 +3133,9 @@
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A98" s="16"/>
+      <c r="A98" s="16" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A99" s="16"/>
@@ -3211,7 +3216,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>